<commit_message>
Add prognosis, update plots for new data
</commit_message>
<xml_diff>
--- a/data/Folkhalsomyndigheten_Covid19.xlsx
+++ b/data/Folkhalsomyndigheten_Covid19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="8270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM 30 Apr 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 11 May 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,14 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W88"/>
+  <dimension ref="A1:W99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="11.90625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -4374,7 +4371,7 @@
         <v>8</v>
       </c>
       <c r="I55" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J55" s="2">
         <v>1</v>
@@ -4416,7 +4413,7 @@
         <v>8</v>
       </c>
       <c r="W55" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:23">
@@ -4495,7 +4492,7 @@
         <v>43920</v>
       </c>
       <c r="B57" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -4531,7 +4528,7 @@
         <v>5</v>
       </c>
       <c r="N57" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O57" s="2">
         <v>60</v>
@@ -4717,7 +4714,7 @@
         <v>6</v>
       </c>
       <c r="E60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="2">
         <v>17</v>
@@ -4744,7 +4741,7 @@
         <v>8</v>
       </c>
       <c r="N60" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O60" s="2">
         <v>34</v>
@@ -5134,7 +5131,7 @@
         <v>43929</v>
       </c>
       <c r="B66" s="2">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C66" s="2">
         <v>2</v>
@@ -5194,7 +5191,7 @@
         <v>68</v>
       </c>
       <c r="V66" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W66" s="2">
         <v>57</v>
@@ -5383,7 +5380,7 @@
         <v>6</v>
       </c>
       <c r="N69" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O69" s="2">
         <v>22</v>
@@ -5410,7 +5407,7 @@
         <v>13</v>
       </c>
       <c r="W69" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" spans="1:23">
@@ -5560,7 +5557,7 @@
         <v>43935</v>
       </c>
       <c r="B72" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -5620,7 +5617,7 @@
         <v>63</v>
       </c>
       <c r="V72" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W72" s="2">
         <v>23</v>
@@ -5986,7 +5983,7 @@
         <v>43941</v>
       </c>
       <c r="B78" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
@@ -6022,7 +6019,7 @@
         <v>9</v>
       </c>
       <c r="N78" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O78" s="2">
         <v>14</v>
@@ -6128,7 +6125,7 @@
         <v>43943</v>
       </c>
       <c r="B80" s="2">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C80" s="2">
         <v>6</v>
@@ -6182,7 +6179,7 @@
         <v>4</v>
       </c>
       <c r="T80" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U80" s="2">
         <v>79</v>
@@ -6199,13 +6196,13 @@
         <v>43944</v>
       </c>
       <c r="B81" s="2">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="C81" s="2">
         <v>2</v>
       </c>
       <c r="D81" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E81" s="2">
         <v>2</v>
@@ -6214,7 +6211,7 @@
         <v>13</v>
       </c>
       <c r="G81" s="2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H81" s="2">
         <v>8</v>
@@ -6270,7 +6267,7 @@
         <v>43945</v>
       </c>
       <c r="B82" s="2">
-        <v>769</v>
+        <v>777</v>
       </c>
       <c r="C82" s="2">
         <v>7</v>
@@ -6285,7 +6282,7 @@
         <v>19</v>
       </c>
       <c r="G82" s="2">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H82" s="2">
         <v>10</v>
@@ -6324,7 +6321,7 @@
         <v>16</v>
       </c>
       <c r="T82" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U82" s="2">
         <v>147</v>
@@ -6356,7 +6353,7 @@
         <v>23</v>
       </c>
       <c r="G83" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H83" s="2">
         <v>13</v>
@@ -6377,7 +6374,7 @@
         <v>12</v>
       </c>
       <c r="N83" s="2">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O83" s="2">
         <v>8</v>
@@ -6412,7 +6409,7 @@
         <v>43947</v>
       </c>
       <c r="B84" s="2">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C84" s="2">
         <v>1</v>
@@ -6427,7 +6424,7 @@
         <v>6</v>
       </c>
       <c r="G84" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H84" s="2">
         <v>1</v>
@@ -6483,7 +6480,7 @@
         <v>43948</v>
       </c>
       <c r="B85" s="2">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="C85" s="2">
         <v>0</v>
@@ -6498,7 +6495,7 @@
         <v>11</v>
       </c>
       <c r="G85" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H85" s="2">
         <v>6</v>
@@ -6519,7 +6516,7 @@
         <v>34</v>
       </c>
       <c r="N85" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="O85" s="2">
         <v>10</v>
@@ -6540,7 +6537,7 @@
         <v>24</v>
       </c>
       <c r="U85" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V85" s="2">
         <v>18</v>
@@ -6554,7 +6551,7 @@
         <v>43949</v>
       </c>
       <c r="B86" s="2">
-        <v>750</v>
+        <v>726</v>
       </c>
       <c r="C86" s="2">
         <v>3</v>
@@ -6569,7 +6566,7 @@
         <v>16</v>
       </c>
       <c r="G86" s="2">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="H86" s="2">
         <v>11</v>
@@ -6587,10 +6584,10 @@
         <v>1</v>
       </c>
       <c r="M86" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N86" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O86" s="2">
         <v>58</v>
@@ -6625,7 +6622,7 @@
         <v>43950</v>
       </c>
       <c r="B87" s="2">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="C87" s="2">
         <v>6</v>
@@ -6634,7 +6631,7 @@
         <v>52</v>
       </c>
       <c r="E87" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F87" s="2">
         <v>21</v>
@@ -6661,7 +6658,7 @@
         <v>37</v>
       </c>
       <c r="N87" s="2">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="O87" s="2">
         <v>34</v>
@@ -6696,70 +6693,851 @@
         <v>43951</v>
       </c>
       <c r="B88" s="2">
-        <v>186</v>
+        <v>598</v>
       </c>
       <c r="C88" s="2">
         <v>0</v>
       </c>
       <c r="D88" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E88" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F88" s="2">
+        <v>21</v>
+      </c>
+      <c r="G88" s="2">
+        <v>8</v>
+      </c>
+      <c r="H88" s="2">
+        <v>20</v>
+      </c>
+      <c r="I88" s="2">
+        <v>28</v>
+      </c>
+      <c r="J88" s="2">
+        <v>7</v>
+      </c>
+      <c r="K88" s="2">
+        <v>12</v>
+      </c>
+      <c r="L88" s="2">
+        <v>9</v>
+      </c>
+      <c r="M88" s="2">
+        <v>29</v>
+      </c>
+      <c r="N88" s="2">
+        <v>176</v>
+      </c>
+      <c r="O88" s="2">
+        <v>23</v>
+      </c>
+      <c r="P88" s="2">
+        <v>44</v>
+      </c>
+      <c r="Q88" s="2">
+        <v>9</v>
+      </c>
+      <c r="R88" s="2">
+        <v>5</v>
+      </c>
+      <c r="S88" s="2">
+        <v>19</v>
+      </c>
+      <c r="T88" s="2">
+        <v>14</v>
+      </c>
+      <c r="U88" s="2">
+        <v>96</v>
+      </c>
+      <c r="V88" s="2">
+        <v>44</v>
+      </c>
+      <c r="W88" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23">
+      <c r="A89" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B89" s="2">
+        <v>532</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2">
+        <v>2</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+      <c r="F89" s="2">
+        <v>21</v>
+      </c>
+      <c r="G89" s="2">
+        <v>2</v>
+      </c>
+      <c r="H89" s="2">
+        <v>7</v>
+      </c>
+      <c r="I89" s="2">
+        <v>23</v>
+      </c>
+      <c r="J89" s="2">
+        <v>7</v>
+      </c>
+      <c r="K89" s="2">
+        <v>15</v>
+      </c>
+      <c r="L89" s="2">
+        <v>7</v>
+      </c>
+      <c r="M89" s="2">
+        <v>12</v>
+      </c>
+      <c r="N89" s="2">
+        <v>141</v>
+      </c>
+      <c r="O89" s="2">
+        <v>55</v>
+      </c>
+      <c r="P89" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q89" s="2">
+        <v>13</v>
+      </c>
+      <c r="R89" s="2">
+        <v>2</v>
+      </c>
+      <c r="S89" s="2">
+        <v>9</v>
+      </c>
+      <c r="T89" s="2">
+        <v>20</v>
+      </c>
+      <c r="U89" s="2">
+        <v>123</v>
+      </c>
+      <c r="V89" s="2">
+        <v>34</v>
+      </c>
+      <c r="W89" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23">
+      <c r="A90" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B90" s="2">
+        <v>298</v>
+      </c>
+      <c r="C90" s="2">
+        <v>1</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2">
+        <v>2</v>
+      </c>
+      <c r="F90" s="2">
+        <v>14</v>
+      </c>
+      <c r="G90" s="2">
+        <v>8</v>
+      </c>
+      <c r="H90" s="2">
+        <v>13</v>
+      </c>
+      <c r="I90" s="2">
+        <v>18</v>
+      </c>
+      <c r="J90" s="2">
+        <v>2</v>
+      </c>
+      <c r="K90" s="2">
+        <v>12</v>
+      </c>
+      <c r="L90" s="2">
+        <v>1</v>
+      </c>
+      <c r="M90" s="2">
+        <v>28</v>
+      </c>
+      <c r="N90" s="2">
+        <v>80</v>
+      </c>
+      <c r="O90" s="2">
+        <v>7</v>
+      </c>
+      <c r="P90" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q90" s="2">
+        <v>6</v>
+      </c>
+      <c r="R90" s="2">
         <v>3</v>
       </c>
-      <c r="G88" s="2">
+      <c r="S90" s="2">
+        <v>7</v>
+      </c>
+      <c r="T90" s="2">
+        <v>13</v>
+      </c>
+      <c r="U90" s="2">
+        <v>33</v>
+      </c>
+      <c r="V90" s="2">
+        <v>20</v>
+      </c>
+      <c r="W90" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23">
+      <c r="A91" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B91" s="2">
+        <v>258</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2">
         <v>3</v>
       </c>
-      <c r="H88" s="2">
+      <c r="E91" s="2">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2">
+        <v>8</v>
+      </c>
+      <c r="G91" s="2">
+        <v>2</v>
+      </c>
+      <c r="H91" s="2">
+        <v>6</v>
+      </c>
+      <c r="I91" s="2">
+        <v>7</v>
+      </c>
+      <c r="J91" s="2">
+        <v>1</v>
+      </c>
+      <c r="K91" s="2">
+        <v>10</v>
+      </c>
+      <c r="L91" s="2">
+        <v>1</v>
+      </c>
+      <c r="M91" s="2">
+        <v>6</v>
+      </c>
+      <c r="N91" s="2">
+        <v>124</v>
+      </c>
+      <c r="O91" s="2">
+        <v>1</v>
+      </c>
+      <c r="P91" s="2">
         <v>11</v>
       </c>
-      <c r="I88" s="2">
+      <c r="Q91" s="2">
         <v>3</v>
       </c>
-      <c r="J88" s="2">
-        <v>2</v>
-      </c>
-      <c r="K88" s="2">
-        <v>1</v>
-      </c>
-      <c r="L88" s="2">
-        <v>1</v>
-      </c>
-      <c r="M88" s="2">
-        <v>0</v>
-      </c>
-      <c r="N88" s="2">
-        <v>55</v>
-      </c>
-      <c r="O88" s="2">
+      <c r="R91" s="2">
+        <v>0</v>
+      </c>
+      <c r="S91" s="2">
+        <v>6</v>
+      </c>
+      <c r="T91" s="2">
+        <v>4</v>
+      </c>
+      <c r="U91" s="2">
+        <v>42</v>
+      </c>
+      <c r="V91" s="2">
+        <v>14</v>
+      </c>
+      <c r="W91" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23">
+      <c r="A92" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B92" s="2">
+        <v>459</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2">
+        <v>64</v>
+      </c>
+      <c r="E92" s="2">
+        <v>6</v>
+      </c>
+      <c r="F92" s="2">
+        <v>23</v>
+      </c>
+      <c r="G92" s="2">
+        <v>11</v>
+      </c>
+      <c r="H92" s="2">
+        <v>2</v>
+      </c>
+      <c r="I92" s="2">
         <v>16</v>
       </c>
-      <c r="P88" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q88" s="2">
+      <c r="J92" s="2">
+        <v>14</v>
+      </c>
+      <c r="K92" s="2">
+        <v>4</v>
+      </c>
+      <c r="L92" s="2">
+        <v>4</v>
+      </c>
+      <c r="M92" s="2">
+        <v>38</v>
+      </c>
+      <c r="N92" s="2">
+        <v>129</v>
+      </c>
+      <c r="O92" s="2">
         <v>3</v>
       </c>
-      <c r="R88" s="2">
-        <v>2</v>
-      </c>
-      <c r="S88" s="2">
-        <v>2</v>
-      </c>
-      <c r="T88" s="2">
+      <c r="P92" s="2">
+        <v>21</v>
+      </c>
+      <c r="Q92" s="2">
+        <v>6</v>
+      </c>
+      <c r="R92" s="2">
+        <v>1</v>
+      </c>
+      <c r="S92" s="2">
+        <v>4</v>
+      </c>
+      <c r="T92" s="2">
+        <v>8</v>
+      </c>
+      <c r="U92" s="2">
+        <v>75</v>
+      </c>
+      <c r="V92" s="2">
+        <v>17</v>
+      </c>
+      <c r="W92" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23">
+      <c r="A93" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B93" s="2">
+        <v>637</v>
+      </c>
+      <c r="C93" s="2">
+        <v>3</v>
+      </c>
+      <c r="D93" s="2">
+        <v>28</v>
+      </c>
+      <c r="E93" s="2">
+        <v>0</v>
+      </c>
+      <c r="F93" s="2">
+        <v>14</v>
+      </c>
+      <c r="G93" s="2">
+        <v>21</v>
+      </c>
+      <c r="H93" s="2">
+        <v>22</v>
+      </c>
+      <c r="I93" s="2">
+        <v>22</v>
+      </c>
+      <c r="J93" s="2">
+        <v>5</v>
+      </c>
+      <c r="K93" s="2">
+        <v>34</v>
+      </c>
+      <c r="L93" s="2">
+        <v>7</v>
+      </c>
+      <c r="M93" s="2">
+        <v>21</v>
+      </c>
+      <c r="N93" s="2">
+        <v>148</v>
+      </c>
+      <c r="O93" s="2">
+        <v>39</v>
+      </c>
+      <c r="P93" s="2">
+        <v>52</v>
+      </c>
+      <c r="Q93" s="2">
+        <v>17</v>
+      </c>
+      <c r="R93" s="2">
+        <v>3</v>
+      </c>
+      <c r="S93" s="2">
+        <v>4</v>
+      </c>
+      <c r="T93" s="2">
+        <v>17</v>
+      </c>
+      <c r="U93" s="2">
+        <v>110</v>
+      </c>
+      <c r="V93" s="2">
+        <v>49</v>
+      </c>
+      <c r="W93" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23">
+      <c r="A94" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B94" s="2">
+        <v>730</v>
+      </c>
+      <c r="C94" s="2">
+        <v>1</v>
+      </c>
+      <c r="D94" s="2">
+        <v>22</v>
+      </c>
+      <c r="E94" s="2">
+        <v>0</v>
+      </c>
+      <c r="F94" s="2">
+        <v>23</v>
+      </c>
+      <c r="G94" s="2">
+        <v>23</v>
+      </c>
+      <c r="H94" s="2">
+        <v>9</v>
+      </c>
+      <c r="I94" s="2">
+        <v>24</v>
+      </c>
+      <c r="J94" s="2">
+        <v>3</v>
+      </c>
+      <c r="K94" s="2">
+        <v>22</v>
+      </c>
+      <c r="L94" s="2">
+        <v>8</v>
+      </c>
+      <c r="M94" s="2">
+        <v>42</v>
+      </c>
+      <c r="N94" s="2">
+        <v>190</v>
+      </c>
+      <c r="O94" s="2">
+        <v>34</v>
+      </c>
+      <c r="P94" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q94" s="2">
+        <v>14</v>
+      </c>
+      <c r="R94" s="2">
+        <v>8</v>
+      </c>
+      <c r="S94" s="2">
+        <v>17</v>
+      </c>
+      <c r="T94" s="2">
+        <v>19</v>
+      </c>
+      <c r="U94" s="2">
+        <v>177</v>
+      </c>
+      <c r="V94" s="2">
+        <v>35</v>
+      </c>
+      <c r="W94" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23">
+      <c r="A95" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B95" s="2">
+        <v>751</v>
+      </c>
+      <c r="C95" s="2">
+        <v>2</v>
+      </c>
+      <c r="D95" s="2">
+        <v>19</v>
+      </c>
+      <c r="E95" s="2">
+        <v>2</v>
+      </c>
+      <c r="F95" s="2">
+        <v>36</v>
+      </c>
+      <c r="G95" s="2">
+        <v>15</v>
+      </c>
+      <c r="H95" s="2">
+        <v>18</v>
+      </c>
+      <c r="I95" s="2">
+        <v>28</v>
+      </c>
+      <c r="J95" s="2">
+        <v>8</v>
+      </c>
+      <c r="K95" s="2">
+        <v>34</v>
+      </c>
+      <c r="L95" s="2">
+        <v>5</v>
+      </c>
+      <c r="M95" s="2">
+        <v>13</v>
+      </c>
+      <c r="N95" s="2">
+        <v>234</v>
+      </c>
+      <c r="O95" s="2">
+        <v>20</v>
+      </c>
+      <c r="P95" s="2">
+        <v>42</v>
+      </c>
+      <c r="Q95" s="2">
+        <v>9</v>
+      </c>
+      <c r="R95" s="2">
+        <v>8</v>
+      </c>
+      <c r="S95" s="2">
+        <v>25</v>
+      </c>
+      <c r="T95" s="2">
+        <v>17</v>
+      </c>
+      <c r="U95" s="2">
+        <v>163</v>
+      </c>
+      <c r="V95" s="2">
+        <v>37</v>
+      </c>
+      <c r="W95" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23">
+      <c r="A96" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B96" s="2">
+        <v>686</v>
+      </c>
+      <c r="C96" s="2">
+        <v>4</v>
+      </c>
+      <c r="D96" s="2">
+        <v>16</v>
+      </c>
+      <c r="E96" s="2">
+        <v>1</v>
+      </c>
+      <c r="F96" s="2">
+        <v>23</v>
+      </c>
+      <c r="G96" s="2">
+        <v>15</v>
+      </c>
+      <c r="H96" s="2">
+        <v>10</v>
+      </c>
+      <c r="I96" s="2">
+        <v>27</v>
+      </c>
+      <c r="J96" s="2">
+        <v>5</v>
+      </c>
+      <c r="K96" s="2">
+        <v>26</v>
+      </c>
+      <c r="L96" s="2">
+        <v>4</v>
+      </c>
+      <c r="M96" s="2">
+        <v>52</v>
+      </c>
+      <c r="N96" s="2">
+        <v>206</v>
+      </c>
+      <c r="O96" s="2">
+        <v>23</v>
+      </c>
+      <c r="P96" s="2">
+        <v>43</v>
+      </c>
+      <c r="Q96" s="2">
+        <v>8</v>
+      </c>
+      <c r="R96" s="2">
+        <v>5</v>
+      </c>
+      <c r="S96" s="2">
+        <v>10</v>
+      </c>
+      <c r="T96" s="2">
+        <v>21</v>
+      </c>
+      <c r="U96" s="2">
+        <v>131</v>
+      </c>
+      <c r="V96" s="2">
+        <v>35</v>
+      </c>
+      <c r="W96" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23">
+      <c r="A97" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B97" s="2">
+        <v>509</v>
+      </c>
+      <c r="C97" s="2">
+        <v>1</v>
+      </c>
+      <c r="D97" s="2">
+        <v>11</v>
+      </c>
+      <c r="E97" s="2">
+        <v>1</v>
+      </c>
+      <c r="F97" s="2">
+        <v>51</v>
+      </c>
+      <c r="G97" s="2">
+        <v>5</v>
+      </c>
+      <c r="H97" s="2">
+        <v>19</v>
+      </c>
+      <c r="I97" s="2">
+        <v>33</v>
+      </c>
+      <c r="J97" s="2">
+        <v>4</v>
+      </c>
+      <c r="K97" s="2">
+        <v>21</v>
+      </c>
+      <c r="L97" s="2">
+        <v>0</v>
+      </c>
+      <c r="M97" s="2">
+        <v>18</v>
+      </c>
+      <c r="N97" s="2">
+        <v>114</v>
+      </c>
+      <c r="O97" s="2">
+        <v>7</v>
+      </c>
+      <c r="P97" s="2">
+        <v>41</v>
+      </c>
+      <c r="Q97" s="2">
+        <v>7</v>
+      </c>
+      <c r="R97" s="2">
+        <v>9</v>
+      </c>
+      <c r="S97" s="2">
+        <v>7</v>
+      </c>
+      <c r="T97" s="2">
+        <v>0</v>
+      </c>
+      <c r="U97" s="2">
+        <v>109</v>
+      </c>
+      <c r="V97" s="2">
+        <v>29</v>
+      </c>
+      <c r="W97" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23">
+      <c r="A98" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B98" s="2">
+        <v>220</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0</v>
+      </c>
+      <c r="D98" s="2">
+        <v>4</v>
+      </c>
+      <c r="E98" s="2">
+        <v>0</v>
+      </c>
+      <c r="F98" s="2">
+        <v>3</v>
+      </c>
+      <c r="G98" s="2">
+        <v>4</v>
+      </c>
+      <c r="H98" s="2">
+        <v>0</v>
+      </c>
+      <c r="I98" s="2">
+        <v>2</v>
+      </c>
+      <c r="J98" s="2">
+        <v>4</v>
+      </c>
+      <c r="K98" s="2">
+        <v>0</v>
+      </c>
+      <c r="L98" s="2">
+        <v>2</v>
+      </c>
+      <c r="M98" s="2">
+        <v>19</v>
+      </c>
+      <c r="N98" s="2">
+        <v>61</v>
+      </c>
+      <c r="O98" s="2">
+        <v>1</v>
+      </c>
+      <c r="P98" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q98" s="2">
+        <v>3</v>
+      </c>
+      <c r="R98" s="2">
+        <v>1</v>
+      </c>
+      <c r="S98" s="2">
+        <v>10</v>
+      </c>
+      <c r="T98" s="2">
+        <v>1</v>
+      </c>
+      <c r="U98" s="2">
+        <v>81</v>
+      </c>
+      <c r="V98" s="2">
+        <v>8</v>
+      </c>
+      <c r="W98" s="2">
         <v>12</v>
       </c>
-      <c r="U88" s="2">
-        <v>41</v>
-      </c>
-      <c r="V88" s="2">
-        <v>17</v>
-      </c>
-      <c r="W88" s="2">
-        <v>13</v>
+    </row>
+    <row r="99" spans="1:23">
+      <c r="A99" s="1">
+        <v>43962</v>
+      </c>
+      <c r="B99" s="2">
+        <v>80</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2">
+        <v>0</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0</v>
+      </c>
+      <c r="G99" s="2">
+        <v>2</v>
+      </c>
+      <c r="H99" s="2">
+        <v>8</v>
+      </c>
+      <c r="I99" s="2">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2">
+        <v>1</v>
+      </c>
+      <c r="K99" s="2">
+        <v>0</v>
+      </c>
+      <c r="L99" s="2">
+        <v>4</v>
+      </c>
+      <c r="M99" s="2">
+        <v>1</v>
+      </c>
+      <c r="N99" s="2">
+        <v>22</v>
+      </c>
+      <c r="O99" s="2">
+        <v>0</v>
+      </c>
+      <c r="P99" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="2">
+        <v>0</v>
+      </c>
+      <c r="R99" s="2">
+        <v>0</v>
+      </c>
+      <c r="S99" s="2">
+        <v>0</v>
+      </c>
+      <c r="T99" s="2">
+        <v>30</v>
+      </c>
+      <c r="U99" s="2">
+        <v>3</v>
+      </c>
+      <c r="V99" s="2">
+        <v>3</v>
+      </c>
+      <c r="W99" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6769,14 +7547,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6879,7 +7656,7 @@
         <v>43912</v>
       </c>
       <c r="B13" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6935,7 +7712,7 @@
         <v>43919</v>
       </c>
       <c r="B20" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -6943,7 +7720,7 @@
         <v>43920</v>
       </c>
       <c r="B21" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -6983,7 +7760,7 @@
         <v>43925</v>
       </c>
       <c r="B26" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -7007,7 +7784,7 @@
         <v>43928</v>
       </c>
       <c r="B29" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -7015,7 +7792,7 @@
         <v>43929</v>
       </c>
       <c r="B30" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -7031,7 +7808,7 @@
         <v>43931</v>
       </c>
       <c r="B32" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -7039,7 +7816,7 @@
         <v>43932</v>
       </c>
       <c r="B33" s="2">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -7047,7 +7824,7 @@
         <v>43933</v>
       </c>
       <c r="B34" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -7071,7 +7848,7 @@
         <v>43936</v>
       </c>
       <c r="B37" s="2">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -7079,7 +7856,7 @@
         <v>43937</v>
       </c>
       <c r="B38" s="2">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -7087,7 +7864,7 @@
         <v>43938</v>
       </c>
       <c r="B39" s="2">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -7095,7 +7872,7 @@
         <v>43939</v>
       </c>
       <c r="B40" s="2">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -7103,7 +7880,7 @@
         <v>43940</v>
       </c>
       <c r="B41" s="2">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -7111,7 +7888,7 @@
         <v>43941</v>
       </c>
       <c r="B42" s="2">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -7119,7 +7896,7 @@
         <v>43942</v>
       </c>
       <c r="B43" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -7127,7 +7904,7 @@
         <v>43943</v>
       </c>
       <c r="B44" s="2">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -7135,7 +7912,7 @@
         <v>43944</v>
       </c>
       <c r="B45" s="2">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -7143,7 +7920,7 @@
         <v>43945</v>
       </c>
       <c r="B46" s="2">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -7151,7 +7928,7 @@
         <v>43946</v>
       </c>
       <c r="B47" s="2">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -7159,7 +7936,7 @@
         <v>43947</v>
       </c>
       <c r="B48" s="2">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -7167,7 +7944,7 @@
         <v>43948</v>
       </c>
       <c r="B49" s="2">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -7175,7 +7952,7 @@
         <v>43949</v>
       </c>
       <c r="B50" s="2">
-        <v>34</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -7183,7 +7960,7 @@
         <v>43950</v>
       </c>
       <c r="B51" s="2">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -7191,15 +7968,103 @@
         <v>43951</v>
       </c>
       <c r="B52" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B53" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B54" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B55" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B56" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B57" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B58" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B59" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B60" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B61" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B62" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="1" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>43962</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="2">
-        <v>10</v>
+      <c r="B64" s="2">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -7209,16 +8074,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -7345,7 +8205,7 @@
         <v>43910</v>
       </c>
       <c r="B16" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -7361,7 +8221,7 @@
         <v>43912</v>
       </c>
       <c r="B18" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -7369,7 +8229,7 @@
         <v>43913</v>
       </c>
       <c r="B19" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -7377,7 +8237,7 @@
         <v>43914</v>
       </c>
       <c r="B20" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -7385,7 +8245,7 @@
         <v>43915</v>
       </c>
       <c r="B21" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -7417,7 +8277,7 @@
         <v>43919</v>
       </c>
       <c r="B25" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -7441,7 +8301,7 @@
         <v>43922</v>
       </c>
       <c r="B28" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -7449,7 +8309,7 @@
         <v>43923</v>
       </c>
       <c r="B29" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -7465,7 +8325,7 @@
         <v>43925</v>
       </c>
       <c r="B31" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -7473,7 +8333,7 @@
         <v>43926</v>
       </c>
       <c r="B32" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -7481,7 +8341,7 @@
         <v>43927</v>
       </c>
       <c r="B33" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -7497,7 +8357,7 @@
         <v>43929</v>
       </c>
       <c r="B35" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -7521,7 +8381,7 @@
         <v>43932</v>
       </c>
       <c r="B38" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -7529,7 +8389,7 @@
         <v>43933</v>
       </c>
       <c r="B39" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -7537,7 +8397,7 @@
         <v>43934</v>
       </c>
       <c r="B40" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -7545,7 +8405,7 @@
         <v>43935</v>
       </c>
       <c r="B41" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -7561,7 +8421,7 @@
         <v>43937</v>
       </c>
       <c r="B43" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -7569,7 +8429,7 @@
         <v>43938</v>
       </c>
       <c r="B44" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -7585,7 +8445,7 @@
         <v>43940</v>
       </c>
       <c r="B46" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -7617,7 +8477,7 @@
         <v>43944</v>
       </c>
       <c r="B50" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -7625,7 +8485,7 @@
         <v>43945</v>
       </c>
       <c r="B51" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -7633,7 +8493,7 @@
         <v>43946</v>
       </c>
       <c r="B52" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -7649,7 +8509,7 @@
         <v>43948</v>
       </c>
       <c r="B54" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -7657,7 +8517,7 @@
         <v>43949</v>
       </c>
       <c r="B55" s="2">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -7665,7 +8525,7 @@
         <v>43950</v>
       </c>
       <c r="B56" s="2">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -7673,6 +8533,94 @@
         <v>43951</v>
       </c>
       <c r="B57" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B58" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B59" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B60" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B61" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B62" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B63" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B64" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B65" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B66" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B67" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>43962</v>
+      </c>
+      <c r="B68" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7685,11 +8633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -7713,10 +8659,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2">
-        <v>45.737628936767578</v>
+        <v>53.256141662597656</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -7730,16 +8676,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>784</v>
+        <v>967</v>
       </c>
       <c r="C3" s="2">
-        <v>272.25436401367188</v>
+        <v>335.80352783203125</v>
       </c>
       <c r="D3" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7747,16 +8693,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2">
-        <v>77.069999694824219</v>
+        <v>107.22782897949219</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7764,16 +8710,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>571</v>
+        <v>805</v>
       </c>
       <c r="C5" s="2">
-        <v>198.69024658203125</v>
+        <v>280.11495971679688</v>
       </c>
       <c r="D5" s="2">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2">
-        <v>55</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7781,16 +8727,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>366</v>
+        <v>479</v>
       </c>
       <c r="C6" s="2">
-        <v>109.63072967529297</v>
+        <v>143.47846984863281</v>
       </c>
       <c r="D6" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7798,16 +8744,16 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>322</v>
+        <v>445</v>
       </c>
       <c r="C7" s="2">
-        <v>246.15855407714844</v>
+        <v>340.18804931640625</v>
       </c>
       <c r="D7" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -7815,16 +8761,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>772</v>
+        <v>998</v>
       </c>
       <c r="C8" s="2">
-        <v>212.32182312011719</v>
+        <v>274.47821044921875</v>
       </c>
       <c r="D8" s="2">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2">
-        <v>67</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -7832,16 +8778,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>167</v>
+        <v>226</v>
       </c>
       <c r="C9" s="2">
-        <v>68.039405822753906</v>
+        <v>92.077278137207031</v>
       </c>
       <c r="D9" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -7849,16 +8795,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>306</v>
+        <v>495</v>
       </c>
       <c r="C10" s="2">
-        <v>151.88441467285156</v>
+        <v>245.69537353515625</v>
       </c>
       <c r="D10" s="2">
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7866,16 +8812,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="C11" s="2">
-        <v>100.76251983642578</v>
+        <v>121.15493011474609</v>
       </c>
       <c r="D11" s="2">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -7883,16 +8829,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>783</v>
+        <v>1061</v>
       </c>
       <c r="C12" s="2">
-        <v>56.82861328125</v>
+        <v>77.00531005859375</v>
       </c>
       <c r="D12" s="2">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E12" s="2">
-        <v>69</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7900,16 +8846,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>8033</v>
+        <v>9607</v>
       </c>
       <c r="C13" s="2">
-        <v>337.93548583984375</v>
+        <v>404.15115356445313</v>
       </c>
       <c r="D13" s="2">
-        <v>593</v>
+        <v>682</v>
       </c>
       <c r="E13" s="2">
-        <v>1406</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -7917,16 +8863,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1215</v>
+        <v>1412</v>
       </c>
       <c r="C14" s="2">
-        <v>408.34844970703125</v>
+        <v>474.55804443359375</v>
       </c>
       <c r="D14" s="2">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E14" s="2">
-        <v>165</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -7934,16 +8880,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>988</v>
+        <v>1309</v>
       </c>
       <c r="C15" s="2">
-        <v>257.48410034179688</v>
+        <v>341.140380859375</v>
       </c>
       <c r="D15" s="2">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="E15" s="2">
-        <v>94</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7951,16 +8897,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>179</v>
+        <v>271</v>
       </c>
       <c r="C16" s="2">
-        <v>63.382125854492188</v>
+        <v>95.958412170410156</v>
       </c>
       <c r="D16" s="2">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7968,16 +8914,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>322</v>
+        <v>365</v>
       </c>
       <c r="C17" s="2">
-        <v>118.49736785888672</v>
+        <v>134.32154846191406</v>
       </c>
       <c r="D17" s="2">
         <v>24</v>
       </c>
       <c r="E17" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7985,16 +8931,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>235</v>
+        <v>351</v>
       </c>
       <c r="C18" s="2">
-        <v>95.782707214355469</v>
+        <v>143.06268310546875</v>
       </c>
       <c r="D18" s="2">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E18" s="2">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -8002,16 +8948,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>766</v>
+        <v>918</v>
       </c>
       <c r="C19" s="2">
-        <v>277.69216918945313</v>
+        <v>332.79559326171875</v>
       </c>
       <c r="D19" s="2">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -8019,16 +8965,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>2459</v>
+        <v>3560</v>
       </c>
       <c r="C20" s="2">
-        <v>142.47795104980469</v>
+        <v>206.27146911621094</v>
       </c>
       <c r="D20" s="2">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="E20" s="2">
-        <v>209</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -8036,16 +8982,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1013</v>
+        <v>1323</v>
       </c>
       <c r="C21" s="2">
-        <v>332.3436279296875</v>
+        <v>434.04800415039063</v>
       </c>
       <c r="D21" s="2">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2">
-        <v>61</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -8053,16 +8999,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>1440</v>
+        <v>1626</v>
       </c>
       <c r="C22" s="2">
-        <v>309.34811401367188</v>
+        <v>349.30557250976563</v>
       </c>
       <c r="D22" s="2">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E22" s="2">
-        <v>102</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -8074,11 +9020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -8099,13 +9043,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>9327</v>
+        <v>11387</v>
       </c>
       <c r="C2" s="2">
-        <v>1103</v>
+        <v>1296</v>
       </c>
       <c r="D2" s="2">
-        <v>1466</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8113,13 +9057,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>11762</v>
+        <v>15280</v>
       </c>
       <c r="C3" s="2">
-        <v>373</v>
+        <v>442</v>
       </c>
       <c r="D3" s="2">
-        <v>1120</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8145,11 +9089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -8170,13 +9112,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8184,7 +9126,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>245</v>
+        <v>293</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -8198,13 +9140,13 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>1630</v>
+        <v>2230</v>
       </c>
       <c r="C4" s="2">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8212,13 +9154,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>2189</v>
+        <v>2927</v>
       </c>
       <c r="C5" s="2">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D5" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8226,13 +9168,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>2814</v>
+        <v>3659</v>
       </c>
       <c r="C6" s="2">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="D6" s="2">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -8240,13 +9182,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>3717</v>
+        <v>4721</v>
       </c>
       <c r="C7" s="2">
-        <v>380</v>
+        <v>458</v>
       </c>
       <c r="D7" s="2">
-        <v>86</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -8254,13 +9196,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>2732</v>
+        <v>3323</v>
       </c>
       <c r="C8" s="2">
-        <v>451</v>
+        <v>526</v>
       </c>
       <c r="D8" s="2">
-        <v>197</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8268,13 +9210,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>2668</v>
+        <v>3221</v>
       </c>
       <c r="C9" s="2">
-        <v>284</v>
+        <v>329</v>
       </c>
       <c r="D9" s="2">
-        <v>596</v>
+        <v>736</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -8282,13 +9224,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>3253</v>
+        <v>3991</v>
       </c>
       <c r="C10" s="2">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2">
-        <v>1048</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -8296,13 +9238,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>1733</v>
+        <v>2170</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>618</v>
+        <v>797</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -8310,7 +9252,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -8330,7 +9272,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Update the data, generate fresh plots, clean-up
</commit_message>
<xml_diff>
--- a/data/Folkhalsomyndigheten_Covid19.xlsx
+++ b/data/Folkhalsomyndigheten_Covid19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="6870" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM 11 May 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 16 May 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -505,11 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W99"/>
+  <dimension ref="A1:W104"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -5007,7 +5011,7 @@
         <v>10</v>
       </c>
       <c r="H64" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I64" s="2">
         <v>10</v>
@@ -5028,7 +5032,7 @@
         <v>131</v>
       </c>
       <c r="O64" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P64" s="2">
         <v>31</v>
@@ -6693,7 +6697,7 @@
         <v>43951</v>
       </c>
       <c r="B88" s="2">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C88" s="2">
         <v>0</v>
@@ -6750,7 +6754,7 @@
         <v>14</v>
       </c>
       <c r="U88" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V88" s="2">
         <v>44</v>
@@ -7119,7 +7123,7 @@
         <v>43957</v>
       </c>
       <c r="B94" s="2">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C94" s="2">
         <v>1</v>
@@ -7152,7 +7156,7 @@
         <v>8</v>
       </c>
       <c r="M94" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N94" s="2">
         <v>190</v>
@@ -7261,7 +7265,7 @@
         <v>43959</v>
       </c>
       <c r="B96" s="2">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C96" s="2">
         <v>4</v>
@@ -7318,7 +7322,7 @@
         <v>21</v>
       </c>
       <c r="U96" s="2">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V96" s="2">
         <v>35</v>
@@ -7403,7 +7407,7 @@
         <v>43961</v>
       </c>
       <c r="B98" s="2">
-        <v>220</v>
+        <v>278</v>
       </c>
       <c r="C98" s="2">
         <v>0</v>
@@ -7415,7 +7419,7 @@
         <v>0</v>
       </c>
       <c r="F98" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G98" s="2">
         <v>4</v>
@@ -7424,28 +7428,28 @@
         <v>0</v>
       </c>
       <c r="I98" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J98" s="2">
         <v>4</v>
       </c>
       <c r="K98" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L98" s="2">
         <v>2</v>
       </c>
       <c r="M98" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N98" s="2">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="O98" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P98" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="Q98" s="2">
         <v>3</v>
@@ -7460,13 +7464,13 @@
         <v>1</v>
       </c>
       <c r="U98" s="2">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="V98" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="W98" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:23">
@@ -7474,70 +7478,425 @@
         <v>43962</v>
       </c>
       <c r="B99" s="2">
-        <v>80</v>
+        <v>411</v>
       </c>
       <c r="C99" s="2">
         <v>0</v>
       </c>
       <c r="D99" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E99" s="2">
         <v>0</v>
       </c>
       <c r="F99" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G99" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H99" s="2">
+        <v>14</v>
+      </c>
+      <c r="I99" s="2">
+        <v>11</v>
+      </c>
+      <c r="J99" s="2">
+        <v>6</v>
+      </c>
+      <c r="K99" s="2">
+        <v>6</v>
+      </c>
+      <c r="L99" s="2">
+        <v>11</v>
+      </c>
+      <c r="M99" s="2">
+        <v>21</v>
+      </c>
+      <c r="N99" s="2">
+        <v>166</v>
+      </c>
+      <c r="O99" s="2">
+        <v>1</v>
+      </c>
+      <c r="P99" s="2">
+        <v>19</v>
+      </c>
+      <c r="Q99" s="2">
+        <v>3</v>
+      </c>
+      <c r="R99" s="2">
+        <v>1</v>
+      </c>
+      <c r="S99" s="2">
+        <v>4</v>
+      </c>
+      <c r="T99" s="2">
+        <v>32</v>
+      </c>
+      <c r="U99" s="2">
+        <v>54</v>
+      </c>
+      <c r="V99" s="2">
+        <v>27</v>
+      </c>
+      <c r="W99" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23">
+      <c r="A100" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B100" s="2">
+        <v>706</v>
+      </c>
+      <c r="C100" s="2">
+        <v>4</v>
+      </c>
+      <c r="D100" s="2">
+        <v>18</v>
+      </c>
+      <c r="E100" s="2">
+        <v>2</v>
+      </c>
+      <c r="F100" s="2">
+        <v>27</v>
+      </c>
+      <c r="G100" s="2">
+        <v>13</v>
+      </c>
+      <c r="H100" s="2">
+        <v>12</v>
+      </c>
+      <c r="I100" s="2">
+        <v>29</v>
+      </c>
+      <c r="J100" s="2">
+        <v>6</v>
+      </c>
+      <c r="K100" s="2">
+        <v>28</v>
+      </c>
+      <c r="L100" s="2">
+        <v>4</v>
+      </c>
+      <c r="M100" s="2">
+        <v>34</v>
+      </c>
+      <c r="N100" s="2">
+        <v>186</v>
+      </c>
+      <c r="O100" s="2">
+        <v>33</v>
+      </c>
+      <c r="P100" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q100" s="2">
+        <v>15</v>
+      </c>
+      <c r="R100" s="2">
+        <v>10</v>
+      </c>
+      <c r="S100" s="2">
+        <v>19</v>
+      </c>
+      <c r="T100" s="2">
+        <v>10</v>
+      </c>
+      <c r="U100" s="2">
+        <v>150</v>
+      </c>
+      <c r="V100" s="2">
+        <v>46</v>
+      </c>
+      <c r="W100" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23">
+      <c r="A101" s="1">
+        <v>43964</v>
+      </c>
+      <c r="B101" s="2">
+        <v>659</v>
+      </c>
+      <c r="C101" s="2">
+        <v>3</v>
+      </c>
+      <c r="D101" s="2">
+        <v>22</v>
+      </c>
+      <c r="E101" s="2">
+        <v>0</v>
+      </c>
+      <c r="F101" s="2">
+        <v>30</v>
+      </c>
+      <c r="G101" s="2">
+        <v>7</v>
+      </c>
+      <c r="H101" s="2">
+        <v>15</v>
+      </c>
+      <c r="I101" s="2">
+        <v>34</v>
+      </c>
+      <c r="J101" s="2">
+        <v>1</v>
+      </c>
+      <c r="K101" s="2">
+        <v>31</v>
+      </c>
+      <c r="L101" s="2">
+        <v>12</v>
+      </c>
+      <c r="M101" s="2">
+        <v>30</v>
+      </c>
+      <c r="N101" s="2">
+        <v>197</v>
+      </c>
+      <c r="O101" s="2">
+        <v>14</v>
+      </c>
+      <c r="P101" s="2">
+        <v>27</v>
+      </c>
+      <c r="Q101" s="2">
+        <v>6</v>
+      </c>
+      <c r="R101" s="2">
+        <v>7</v>
+      </c>
+      <c r="S101" s="2">
+        <v>15</v>
+      </c>
+      <c r="T101" s="2">
+        <v>26</v>
+      </c>
+      <c r="U101" s="2">
+        <v>133</v>
+      </c>
+      <c r="V101" s="2">
+        <v>30</v>
+      </c>
+      <c r="W101" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23">
+      <c r="A102" s="1">
+        <v>43965</v>
+      </c>
+      <c r="B102" s="2">
+        <v>626</v>
+      </c>
+      <c r="C102" s="2">
+        <v>2</v>
+      </c>
+      <c r="D102" s="2">
+        <v>15</v>
+      </c>
+      <c r="E102" s="2">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2">
+        <v>40</v>
+      </c>
+      <c r="G102" s="2">
+        <v>13</v>
+      </c>
+      <c r="H102" s="2">
+        <v>30</v>
+      </c>
+      <c r="I102" s="2">
+        <v>14</v>
+      </c>
+      <c r="J102" s="2">
+        <v>5</v>
+      </c>
+      <c r="K102" s="2">
+        <v>18</v>
+      </c>
+      <c r="L102" s="2">
+        <v>6</v>
+      </c>
+      <c r="M102" s="2">
+        <v>39</v>
+      </c>
+      <c r="N102" s="2">
+        <v>117</v>
+      </c>
+      <c r="O102" s="2">
+        <v>11</v>
+      </c>
+      <c r="P102" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q102" s="2">
+        <v>14</v>
+      </c>
+      <c r="R102" s="2">
+        <v>14</v>
+      </c>
+      <c r="S102" s="2">
+        <v>14</v>
+      </c>
+      <c r="T102" s="2">
+        <v>31</v>
+      </c>
+      <c r="U102" s="2">
+        <v>151</v>
+      </c>
+      <c r="V102" s="2">
+        <v>24</v>
+      </c>
+      <c r="W102" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23">
+      <c r="A103" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B103" s="2">
+        <v>604</v>
+      </c>
+      <c r="C103" s="2">
+        <v>6</v>
+      </c>
+      <c r="D103" s="2">
+        <v>10</v>
+      </c>
+      <c r="E103" s="2">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2">
+        <v>30</v>
+      </c>
+      <c r="G103" s="2">
+        <v>18</v>
+      </c>
+      <c r="H103" s="2">
+        <v>15</v>
+      </c>
+      <c r="I103" s="2">
+        <v>36</v>
+      </c>
+      <c r="J103" s="2">
+        <v>7</v>
+      </c>
+      <c r="K103" s="2">
         <v>8</v>
       </c>
-      <c r="I99" s="2">
-        <v>0</v>
-      </c>
-      <c r="J99" s="2">
-        <v>1</v>
-      </c>
-      <c r="K99" s="2">
-        <v>0</v>
-      </c>
-      <c r="L99" s="2">
-        <v>4</v>
-      </c>
-      <c r="M99" s="2">
-        <v>1</v>
-      </c>
-      <c r="N99" s="2">
-        <v>22</v>
-      </c>
-      <c r="O99" s="2">
-        <v>0</v>
-      </c>
-      <c r="P99" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q99" s="2">
-        <v>0</v>
-      </c>
-      <c r="R99" s="2">
-        <v>0</v>
-      </c>
-      <c r="S99" s="2">
-        <v>0</v>
-      </c>
-      <c r="T99" s="2">
-        <v>30</v>
-      </c>
-      <c r="U99" s="2">
+      <c r="L103" s="2">
+        <v>1</v>
+      </c>
+      <c r="M103" s="2">
+        <v>37</v>
+      </c>
+      <c r="N103" s="2">
+        <v>141</v>
+      </c>
+      <c r="O103" s="2">
+        <v>17</v>
+      </c>
+      <c r="P103" s="2">
+        <v>23</v>
+      </c>
+      <c r="Q103" s="2">
+        <v>8</v>
+      </c>
+      <c r="R103" s="2">
+        <v>14</v>
+      </c>
+      <c r="S103" s="2">
+        <v>25</v>
+      </c>
+      <c r="T103" s="2">
+        <v>14</v>
+      </c>
+      <c r="U103" s="2">
+        <v>153</v>
+      </c>
+      <c r="V103" s="2">
+        <v>26</v>
+      </c>
+      <c r="W103" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23">
+      <c r="A104" s="1">
+        <v>43967</v>
+      </c>
+      <c r="B104" s="2">
+        <v>26</v>
+      </c>
+      <c r="C104" s="2">
+        <v>0</v>
+      </c>
+      <c r="D104" s="2">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2">
+        <v>0</v>
+      </c>
+      <c r="F104" s="2">
         <v>3</v>
       </c>
-      <c r="V99" s="2">
-        <v>3</v>
-      </c>
-      <c r="W99" s="2">
+      <c r="G104" s="2">
+        <v>0</v>
+      </c>
+      <c r="H104" s="2">
+        <v>0</v>
+      </c>
+      <c r="I104" s="2">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2">
+        <v>0</v>
+      </c>
+      <c r="K104" s="2">
+        <v>0</v>
+      </c>
+      <c r="L104" s="2">
+        <v>0</v>
+      </c>
+      <c r="M104" s="2">
+        <v>1</v>
+      </c>
+      <c r="N104" s="2">
+        <v>16</v>
+      </c>
+      <c r="O104" s="2">
+        <v>0</v>
+      </c>
+      <c r="P104" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="2">
         <v>5</v>
+      </c>
+      <c r="R104" s="2">
+        <v>1</v>
+      </c>
+      <c r="S104" s="2">
+        <v>0</v>
+      </c>
+      <c r="T104" s="2">
+        <v>0</v>
+      </c>
+      <c r="U104" s="2">
+        <v>0</v>
+      </c>
+      <c r="V104" s="2">
+        <v>0</v>
+      </c>
+      <c r="W104" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7547,13 +7906,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -7760,7 +8122,7 @@
         <v>43925</v>
       </c>
       <c r="B26" s="2">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -7784,7 +8146,7 @@
         <v>43928</v>
       </c>
       <c r="B29" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -7832,7 +8194,7 @@
         <v>43934</v>
       </c>
       <c r="B35" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -7848,7 +8210,7 @@
         <v>43936</v>
       </c>
       <c r="B37" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -7872,7 +8234,7 @@
         <v>43939</v>
       </c>
       <c r="B40" s="2">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -7880,7 +8242,7 @@
         <v>43940</v>
       </c>
       <c r="B41" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -7888,7 +8250,7 @@
         <v>43941</v>
       </c>
       <c r="B42" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -7904,7 +8266,7 @@
         <v>43943</v>
       </c>
       <c r="B44" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -7912,7 +8274,7 @@
         <v>43944</v>
       </c>
       <c r="B45" s="2">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -7920,7 +8282,7 @@
         <v>43945</v>
       </c>
       <c r="B46" s="2">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -7928,7 +8290,7 @@
         <v>43946</v>
       </c>
       <c r="B47" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -7936,7 +8298,7 @@
         <v>43947</v>
       </c>
       <c r="B48" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -7944,7 +8306,7 @@
         <v>43948</v>
       </c>
       <c r="B49" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -7952,7 +8314,7 @@
         <v>43949</v>
       </c>
       <c r="B50" s="2">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -7960,7 +8322,7 @@
         <v>43950</v>
       </c>
       <c r="B51" s="2">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -7968,7 +8330,7 @@
         <v>43951</v>
       </c>
       <c r="B52" s="2">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -7976,7 +8338,7 @@
         <v>43952</v>
       </c>
       <c r="B53" s="2">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -7984,7 +8346,7 @@
         <v>43953</v>
       </c>
       <c r="B54" s="2">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -7992,7 +8354,7 @@
         <v>43954</v>
       </c>
       <c r="B55" s="2">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -8000,7 +8362,7 @@
         <v>43955</v>
       </c>
       <c r="B56" s="2">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -8008,7 +8370,7 @@
         <v>43956</v>
       </c>
       <c r="B57" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -8016,7 +8378,7 @@
         <v>43957</v>
       </c>
       <c r="B58" s="2">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -8024,7 +8386,7 @@
         <v>43958</v>
       </c>
       <c r="B59" s="2">
-        <v>32</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -8032,7 +8394,7 @@
         <v>43959</v>
       </c>
       <c r="B60" s="2">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -8040,7 +8402,7 @@
         <v>43960</v>
       </c>
       <c r="B61" s="2">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -8048,7 +8410,7 @@
         <v>43961</v>
       </c>
       <c r="B62" s="2">
-        <v>9</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -8056,15 +8418,47 @@
         <v>43962</v>
       </c>
       <c r="B63" s="2">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B64" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>43964</v>
+      </c>
+      <c r="B65" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>43965</v>
+      </c>
+      <c r="B66" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B67" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="2">
-        <v>14</v>
+      <c r="B68" s="2">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -8074,7 +8468,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8213,7 +8607,7 @@
         <v>43911</v>
       </c>
       <c r="B17" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -8221,7 +8615,7 @@
         <v>43912</v>
       </c>
       <c r="B18" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -8261,7 +8655,7 @@
         <v>43917</v>
       </c>
       <c r="B23" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -8269,7 +8663,7 @@
         <v>43918</v>
       </c>
       <c r="B24" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -8285,7 +8679,7 @@
         <v>43920</v>
       </c>
       <c r="B26" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -8309,7 +8703,7 @@
         <v>43923</v>
       </c>
       <c r="B29" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -8325,7 +8719,7 @@
         <v>43925</v>
       </c>
       <c r="B31" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -8333,7 +8727,7 @@
         <v>43926</v>
       </c>
       <c r="B32" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -8341,7 +8735,7 @@
         <v>43927</v>
       </c>
       <c r="B33" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -8381,7 +8775,7 @@
         <v>43932</v>
       </c>
       <c r="B38" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -8397,7 +8791,7 @@
         <v>43934</v>
       </c>
       <c r="B40" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -8405,7 +8799,7 @@
         <v>43935</v>
       </c>
       <c r="B41" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -8413,7 +8807,7 @@
         <v>43936</v>
       </c>
       <c r="B42" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -8421,7 +8815,7 @@
         <v>43937</v>
       </c>
       <c r="B43" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -8453,7 +8847,7 @@
         <v>43941</v>
       </c>
       <c r="B47" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -8477,7 +8871,7 @@
         <v>43944</v>
       </c>
       <c r="B50" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -8493,7 +8887,7 @@
         <v>43946</v>
       </c>
       <c r="B52" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -8501,7 +8895,7 @@
         <v>43947</v>
       </c>
       <c r="B53" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -8509,7 +8903,7 @@
         <v>43948</v>
       </c>
       <c r="B54" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -8517,7 +8911,7 @@
         <v>43949</v>
       </c>
       <c r="B55" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -8525,7 +8919,7 @@
         <v>43950</v>
       </c>
       <c r="B56" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -8533,7 +8927,7 @@
         <v>43951</v>
       </c>
       <c r="B57" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -8549,7 +8943,7 @@
         <v>43953</v>
       </c>
       <c r="B59" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -8557,7 +8951,7 @@
         <v>43954</v>
       </c>
       <c r="B60" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -8573,7 +8967,7 @@
         <v>43956</v>
       </c>
       <c r="B62" s="2">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -8581,7 +8975,7 @@
         <v>43957</v>
       </c>
       <c r="B63" s="2">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -8589,7 +8983,7 @@
         <v>43958</v>
       </c>
       <c r="B64" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -8597,7 +8991,7 @@
         <v>43959</v>
       </c>
       <c r="B65" s="2">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -8605,7 +8999,7 @@
         <v>43960</v>
       </c>
       <c r="B66" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -8613,7 +9007,7 @@
         <v>43961</v>
       </c>
       <c r="B67" s="2">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -8621,7 +9015,39 @@
         <v>43962</v>
       </c>
       <c r="B68" s="2">
-        <v>4</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B69" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>43964</v>
+      </c>
+      <c r="B70" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>43965</v>
+      </c>
+      <c r="B71" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B72" s="2">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -8633,7 +9059,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -8659,16 +9087,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2">
-        <v>53.256141662597656</v>
+        <v>62.654285430908203</v>
       </c>
       <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
         <v>3</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8676,16 +9104,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>967</v>
+        <v>1035</v>
       </c>
       <c r="C3" s="2">
-        <v>335.80352783203125</v>
+        <v>359.41741943359375</v>
       </c>
       <c r="D3" s="2">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8693,10 +9121,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2">
-        <v>107.22782897949219</v>
+        <v>110.57869720458984</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
@@ -8710,16 +9138,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>805</v>
+        <v>950</v>
       </c>
       <c r="C5" s="2">
-        <v>280.11495971679688</v>
+        <v>330.57046508789063</v>
       </c>
       <c r="D5" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -8727,16 +9155,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>479</v>
+        <v>538</v>
       </c>
       <c r="C6" s="2">
-        <v>143.47846984863281</v>
+        <v>161.15118408203125</v>
       </c>
       <c r="D6" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -8744,16 +9172,16 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>445</v>
+        <v>522</v>
       </c>
       <c r="C7" s="2">
-        <v>340.18804931640625</v>
+        <v>399.05206298828125</v>
       </c>
       <c r="D7" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -8761,16 +9189,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>998</v>
+        <v>1126</v>
       </c>
       <c r="C8" s="2">
-        <v>274.47821044921875</v>
+        <v>309.68182373046875</v>
       </c>
       <c r="D8" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2">
-        <v>96</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -8778,16 +9206,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="C9" s="2">
-        <v>92.077278137207031</v>
+        <v>101.85540008544922</v>
       </c>
       <c r="D9" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -8795,16 +9223,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>495</v>
+        <v>592</v>
       </c>
       <c r="C10" s="2">
-        <v>245.69537353515625</v>
+        <v>293.84173583984375</v>
       </c>
       <c r="D10" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -8812,16 +9240,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>303</v>
+        <v>333</v>
       </c>
       <c r="C11" s="2">
-        <v>121.15493011474609</v>
+        <v>133.15046691894531</v>
       </c>
       <c r="D11" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -8829,16 +9257,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1061</v>
+        <v>1220</v>
       </c>
       <c r="C12" s="2">
-        <v>77.00531005859375</v>
+        <v>88.54522705078125</v>
       </c>
       <c r="D12" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -8846,16 +9274,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>9607</v>
+        <v>10425</v>
       </c>
       <c r="C13" s="2">
-        <v>404.15115356445313</v>
+        <v>438.56307983398438</v>
       </c>
       <c r="D13" s="2">
-        <v>682</v>
+        <v>729</v>
       </c>
       <c r="E13" s="2">
-        <v>1688</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -8863,16 +9291,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1412</v>
+        <v>1494</v>
       </c>
       <c r="C14" s="2">
-        <v>474.55804443359375</v>
+        <v>502.11737060546875</v>
       </c>
       <c r="D14" s="2">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="E14" s="2">
-        <v>188</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -8880,16 +9308,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>1309</v>
+        <v>1452</v>
       </c>
       <c r="C15" s="2">
-        <v>341.140380859375</v>
+        <v>378.40780639648438</v>
       </c>
       <c r="D15" s="2">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2">
-        <v>120</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -8897,16 +9325,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="C16" s="2">
-        <v>95.958412170410156</v>
+        <v>114.01701354980469</v>
       </c>
       <c r="D16" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -8914,16 +9342,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>365</v>
+        <v>412</v>
       </c>
       <c r="C17" s="2">
-        <v>134.32154846191406</v>
+        <v>151.61775207519531</v>
       </c>
       <c r="D17" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -8931,16 +9359,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>351</v>
+        <v>428</v>
       </c>
       <c r="C18" s="2">
-        <v>143.06268310546875</v>
+        <v>174.44680786132813</v>
       </c>
       <c r="D18" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E18" s="2">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -8948,16 +9376,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>918</v>
+        <v>1001</v>
       </c>
       <c r="C19" s="2">
-        <v>332.79559326171875</v>
+        <v>362.88494873046875</v>
       </c>
       <c r="D19" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -8965,16 +9393,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>3560</v>
+        <v>4201</v>
       </c>
       <c r="C20" s="2">
-        <v>206.27146911621094</v>
+        <v>243.41191101074219</v>
       </c>
       <c r="D20" s="2">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="E20" s="2">
-        <v>297</v>
+        <v>385</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -8982,16 +9410,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1323</v>
+        <v>1481</v>
       </c>
       <c r="C21" s="2">
-        <v>434.04800415039063</v>
+        <v>485.88442993164063</v>
       </c>
       <c r="D21" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E21" s="2">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -8999,16 +9427,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>1626</v>
+        <v>1729</v>
       </c>
       <c r="C22" s="2">
-        <v>349.30557250976563</v>
+        <v>371.43255615234375</v>
       </c>
       <c r="D22" s="2">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2">
-        <v>147</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -9020,7 +9448,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -9043,13 +9473,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>11387</v>
+        <v>12423</v>
       </c>
       <c r="C2" s="2">
-        <v>1296</v>
+        <v>1358</v>
       </c>
       <c r="D2" s="2">
-        <v>1827</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9057,13 +9487,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>15280</v>
+        <v>17251</v>
       </c>
       <c r="C3" s="2">
-        <v>442</v>
+        <v>475</v>
       </c>
       <c r="D3" s="2">
-        <v>1429</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -9089,9 +9519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -9112,7 +9548,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -9126,7 +9562,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>293</v>
+        <v>341</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -9140,13 +9576,13 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>2230</v>
+        <v>2563</v>
       </c>
       <c r="C4" s="2">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -9154,13 +9590,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>2927</v>
+        <v>3382</v>
       </c>
       <c r="C5" s="2">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -9168,13 +9604,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>3659</v>
+        <v>4181</v>
       </c>
       <c r="C6" s="2">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D6" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -9182,13 +9618,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>4721</v>
+        <v>5287</v>
       </c>
       <c r="C7" s="2">
-        <v>458</v>
+        <v>484</v>
       </c>
       <c r="D7" s="2">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -9196,13 +9632,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>3323</v>
+        <v>3657</v>
       </c>
       <c r="C8" s="2">
-        <v>526</v>
+        <v>553</v>
       </c>
       <c r="D8" s="2">
-        <v>239</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -9210,13 +9646,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>3221</v>
+        <v>3459</v>
       </c>
       <c r="C9" s="2">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="D9" s="2">
-        <v>736</v>
+        <v>817</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -9224,13 +9660,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>3991</v>
+        <v>4314</v>
       </c>
       <c r="C10" s="2">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2">
-        <v>1329</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -9238,13 +9674,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2170</v>
+        <v>2347</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>797</v>
+        <v>907</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>